<commit_message>
upgrade calculation for multiple variables
</commit_message>
<xml_diff>
--- a/TestData/Results/WithinGroupResults.xlsx
+++ b/TestData/Results/WithinGroupResults.xlsx
@@ -443,7 +443,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,11 +451,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="9.6" customWidth="1" min="1" max="1"/>
-    <col width="20.4" customWidth="1" min="2" max="2"/>
+    <col width="24" customWidth="1" min="1" max="1"/>
+    <col width="21.6" customWidth="1" min="2" max="2"/>
     <col width="21.6" customWidth="1" min="3" max="3"/>
     <col width="22.8" customWidth="1" min="4" max="4"/>
-    <col width="24" customWidth="1" min="5" max="5"/>
+    <col width="25.2" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -492,35 +492,947 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>12.91771146434375</v>
+        <v>3.50657896709375</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>1.784983880385238</v>
+        <v>1.559032477982836</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>-0.7240632086390901</v>
+        <v>-0.4960395974372989</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>0.1836175174327505</v>
+        <v>-0.08409244466413099</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
+          <t>BC-&gt;0--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>1.9696643411875</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>1.182555496582983</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>-0.9291717101703347</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>-0.07406904894674896</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;1--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>3.231586244625</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>1.139879130938501</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>-1.193328255124775</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>-0.009348925600232597</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;2--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>3.948225075375</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>1.205830559298445</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>-1.245976620261673</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>0.007342742065263715</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;3--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>4.8768402071875</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>1.116050425771497</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>-1.220623063030768</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>0.2399775366093591</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>BS-&gt;0--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>2.0373165026875</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>1.212651232212299</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>-0.9913227480710893</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>-0.1484432291517285</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>BS-&gt;1--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>3.0468729508125</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>0.9875061370255511</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>-1.001682886891879</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>-0.1801309704986296</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>BS-&gt;2--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>3.9312273920625</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>1.166060255310559</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>-1.185436403500674</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>-0.4064186056249479</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>BS-&gt;3--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>5.010899022812501</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>1.126410035680396</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>-1.188927001364296</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>-0.09924865272162578</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;0; BS-&gt;0--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>0.404273861</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>0.3854788581458037</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>-1.652374956386593</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>0.2491189435134492</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;0; BS-&gt;1--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>1.71937215675</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>0.3293090874744067</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>-0.8245368825799058</v>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>-0.9013229161711491</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;0; BS-&gt;2--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>2.234526481</v>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>0.1166473631413766</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>-0.9910764732394011</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>-0.2221169382117277</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;0; BS-&gt;3--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>3.520484866</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>0.2654984586473224</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>-1.18308758303635</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>0.05730857881496489</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;1; BS-&gt;0--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>1.7433388585</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>0.2057904418763836</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>-1.615511828308509</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>0.2253509661202346</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;1; BS-&gt;1--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>2.7887344075</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>0.1118460503176008</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>-1.332692544268311</v>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>-0.1391994192074564</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;1; BS-&gt;2--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>3.713800361</v>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>0.1319281902003499</v>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>-0.8313920201503273</v>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>0.9699859316854175</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;1; BS-&gt;3--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>4.6804713515</v>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>0.31722098747118</v>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>-0.8979283529592332</v>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>-0.7773408947687563</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;2; BS-&gt;0--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>2.4289886535</v>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>0.2687085664842178</v>
+      </c>
+      <c r="D19" s="2" t="n">
+        <v>-0.9326403227697027</v>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>-0.5978520435536865</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;2; BS-&gt;1--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>3.395419905</v>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>0.305465367278942</v>
+      </c>
+      <c r="D20" s="2" t="n">
+        <v>-1.02429365032042</v>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>0.648163258395336</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;2; BS-&gt;2--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="n">
+        <v>4.54520676125</v>
+      </c>
+      <c r="C21" s="2" t="n">
+        <v>0.2969784977320904</v>
+      </c>
+      <c r="D21" s="2" t="n">
+        <v>-1.454764585922154</v>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>-0.01424553084629778</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;2; BS-&gt;3--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B22" s="2" t="n">
+        <v>5.42328498175</v>
+      </c>
+      <c r="C22" s="2" t="n">
+        <v>0.3940534389976101</v>
+      </c>
+      <c r="D22" s="2" t="n">
+        <v>-0.9604530831080429</v>
+      </c>
+      <c r="E22" s="2" t="n">
+        <v>0.6249361528795221</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;3; BS-&gt;0--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B23" s="2" t="n">
+        <v>3.57266463775</v>
+      </c>
+      <c r="C23" s="2" t="n">
+        <v>0.2662035173159032</v>
+      </c>
+      <c r="D23" s="2" t="n">
+        <v>-1.67984068960373</v>
+      </c>
+      <c r="E23" s="2" t="n">
+        <v>0.2053451861889831</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;3; BS-&gt;1--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B24" s="2" t="n">
+        <v>4.283965334</v>
+      </c>
+      <c r="C24" s="2" t="n">
+        <v>0.1433301637895081</v>
+      </c>
+      <c r="D24" s="2" t="n">
+        <v>-1.030237760211063</v>
+      </c>
+      <c r="E24" s="2" t="n">
+        <v>0.5405883772942711</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;3; BS-&gt;2--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B25" s="2" t="n">
+        <v>5.231375965</v>
+      </c>
+      <c r="C25" s="2" t="n">
+        <v>0.146198774551496</v>
+      </c>
+      <c r="D25" s="2" t="n">
+        <v>-1.350463078056914</v>
+      </c>
+      <c r="E25" s="2" t="n">
+        <v>0.4828642381594128</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;3; BS-&gt;3--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B26" s="2" t="n">
+        <v>6.419354892</v>
+      </c>
+      <c r="C26" s="2" t="n">
+        <v>0.1962105604206064</v>
+      </c>
+      <c r="D26" s="2" t="n">
+        <v>-1.085957672650951</v>
+      </c>
+      <c r="E26" s="2" t="n">
+        <v>0.6731845983740794</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="inlineStr">
+        <is>
           <t>Speed</t>
         </is>
       </c>
-      <c r="B3" s="2" t="n">
-        <v>13.11623078709375</v>
-      </c>
-      <c r="C3" s="2" t="n">
-        <v>2.651200025119505</v>
-      </c>
-      <c r="D3" s="2" t="n">
-        <v>-1.137678003032307</v>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>-0.04279985824825186</v>
+      <c r="B27" s="2" t="n">
+        <v>17.080398762125</v>
+      </c>
+      <c r="C27" s="2" t="n">
+        <v>11.33185851771384</v>
+      </c>
+      <c r="D27" s="2" t="n">
+        <v>-1.327686773944483</v>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>-0.01063856572013002</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;0--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B28" s="2" t="n">
+        <v>15.642069044625</v>
+      </c>
+      <c r="C28" s="2" t="n">
+        <v>11.53728718241722</v>
+      </c>
+      <c r="D28" s="2" t="n">
+        <v>-1.356440192294449</v>
+      </c>
+      <c r="E28" s="2" t="n">
+        <v>-0.01419490647049016</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;1--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B29" s="2" t="n">
+        <v>16.4778438143125</v>
+      </c>
+      <c r="C29" s="2" t="n">
+        <v>11.54159174314436</v>
+      </c>
+      <c r="D29" s="2" t="n">
+        <v>-1.335649323451923</v>
+      </c>
+      <c r="E29" s="2" t="n">
+        <v>-0.008499795938592795</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;2--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B30" s="2" t="n">
+        <v>17.5213600068125</v>
+      </c>
+      <c r="C30" s="2" t="n">
+        <v>11.55723890964476</v>
+      </c>
+      <c r="D30" s="2" t="n">
+        <v>-1.362450383577653</v>
+      </c>
+      <c r="E30" s="2" t="n">
+        <v>-0.01318813035193363</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;3--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B31" s="2" t="n">
+        <v>18.68032218275</v>
+      </c>
+      <c r="C31" s="2" t="n">
+        <v>11.57183487000701</v>
+      </c>
+      <c r="D31" s="2" t="n">
+        <v>-1.367038852633238</v>
+      </c>
+      <c r="E31" s="2" t="n">
+        <v>-0.01089799399313881</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="inlineStr">
+        <is>
+          <t>BS-&gt;0--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B32" s="2" t="n">
+        <v>2.01539394475</v>
+      </c>
+      <c r="C32" s="2" t="n">
+        <v>1.210668328221953</v>
+      </c>
+      <c r="D32" s="2" t="n">
+        <v>-1.389704897644074</v>
+      </c>
+      <c r="E32" s="2" t="n">
+        <v>0.1775920290921806</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="inlineStr">
+        <is>
+          <t>BS-&gt;1--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B33" s="2" t="n">
+        <v>12.158589275625</v>
+      </c>
+      <c r="C33" s="2" t="n">
+        <v>1.131492254370851</v>
+      </c>
+      <c r="D33" s="2" t="n">
+        <v>-1.293948411330144</v>
+      </c>
+      <c r="E33" s="2" t="n">
+        <v>0.09413575861830703</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="inlineStr">
+        <is>
+          <t>BS-&gt;2--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B34" s="2" t="n">
+        <v>22.109648053125</v>
+      </c>
+      <c r="C34" s="2" t="n">
+        <v>1.263974850210778</v>
+      </c>
+      <c r="D34" s="2" t="n">
+        <v>-1.44058171931666</v>
+      </c>
+      <c r="E34" s="2" t="n">
+        <v>0.2218106033919279</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="inlineStr">
+        <is>
+          <t>BS-&gt;3--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B35" s="2" t="n">
+        <v>32.037963775</v>
+      </c>
+      <c r="C35" s="2" t="n">
+        <v>1.198022624345362</v>
+      </c>
+      <c r="D35" s="2" t="n">
+        <v>-1.208762387188467</v>
+      </c>
+      <c r="E35" s="2" t="n">
+        <v>0.1327243542180619</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;0; BS-&gt;0--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B36" s="2" t="n">
+        <v>0.5827117159999999</v>
+      </c>
+      <c r="C36" s="2" t="n">
+        <v>0.1625307493704574</v>
+      </c>
+      <c r="D36" s="2" t="n">
+        <v>-1.559352460832012</v>
+      </c>
+      <c r="E36" s="2" t="n">
+        <v>-0.2521040923751826</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;0; BS-&gt;1--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B37" s="2" t="n">
+        <v>10.7344552475</v>
+      </c>
+      <c r="C37" s="2" t="n">
+        <v>0.1441027316987529</v>
+      </c>
+      <c r="D37" s="2" t="n">
+        <v>-0.8641240820543454</v>
+      </c>
+      <c r="E37" s="2" t="n">
+        <v>-0.9309825218628531</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;0; BS-&gt;2--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B38" s="2" t="n">
+        <v>20.6847894375</v>
+      </c>
+      <c r="C38" s="2" t="n">
+        <v>0.2202118638344981</v>
+      </c>
+      <c r="D38" s="2" t="n">
+        <v>-0.7730019293786197</v>
+      </c>
+      <c r="E38" s="2" t="n">
+        <v>-0.981206409814895</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;0; BS-&gt;3--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B39" s="2" t="n">
+        <v>30.5663197775</v>
+      </c>
+      <c r="C39" s="2" t="n">
+        <v>0.2726943941279972</v>
+      </c>
+      <c r="D39" s="2" t="n">
+        <v>-1.294278241858982</v>
+      </c>
+      <c r="E39" s="2" t="n">
+        <v>-0.04543732363831735</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;1; BS-&gt;0--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B40" s="2" t="n">
+        <v>1.39177759475</v>
+      </c>
+      <c r="C40" s="2" t="n">
+        <v>0.3380760107216575</v>
+      </c>
+      <c r="D40" s="2" t="n">
+        <v>-1.448404911539488</v>
+      </c>
+      <c r="E40" s="2" t="n">
+        <v>0.4244697311021177</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;1; BS-&gt;1--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B41" s="2" t="n">
+        <v>11.699902555</v>
+      </c>
+      <c r="C41" s="2" t="n">
+        <v>0.2258772345191609</v>
+      </c>
+      <c r="D41" s="2" t="n">
+        <v>-0.9913601409176644</v>
+      </c>
+      <c r="E41" s="2" t="n">
+        <v>-0.3335572666752883</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;1; BS-&gt;2--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B42" s="2" t="n">
+        <v>21.3294006725</v>
+      </c>
+      <c r="C42" s="2" t="n">
+        <v>0.2685776164333116</v>
+      </c>
+      <c r="D42" s="2" t="n">
+        <v>-0.6954722949866068</v>
+      </c>
+      <c r="E42" s="2" t="n">
+        <v>1.113554836938734</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;1; BS-&gt;3--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B43" s="2" t="n">
+        <v>31.490294435</v>
+      </c>
+      <c r="C43" s="2" t="n">
+        <v>0.1781132128129339</v>
+      </c>
+      <c r="D43" s="2" t="n">
+        <v>-0.7439687351966686</v>
+      </c>
+      <c r="E43" s="2" t="n">
+        <v>-1.031648141886174</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;2; BS-&gt;0--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B44" s="2" t="n">
+        <v>2.46759357975</v>
+      </c>
+      <c r="C44" s="2" t="n">
+        <v>0.4313901623750228</v>
+      </c>
+      <c r="D44" s="2" t="n">
+        <v>-1.80212385696959</v>
+      </c>
+      <c r="E44" s="2" t="n">
+        <v>-0.07149254113398355</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;2; BS-&gt;1--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B45" s="2" t="n">
+        <v>12.5414554525</v>
+      </c>
+      <c r="C45" s="2" t="n">
+        <v>0.353739409150169</v>
+      </c>
+      <c r="D45" s="2" t="n">
+        <v>-0.9931476810910591</v>
+      </c>
+      <c r="E45" s="2" t="n">
+        <v>-0.7086112894401293</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;2; BS-&gt;2--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B46" s="2" t="n">
+        <v>22.6185951475</v>
+      </c>
+      <c r="C46" s="2" t="n">
+        <v>0.3740324475967611</v>
+      </c>
+      <c r="D46" s="2" t="n">
+        <v>-1.593711485506129</v>
+      </c>
+      <c r="E46" s="2" t="n">
+        <v>-0.1887314434903983</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;2; BS-&gt;3--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B47" s="2" t="n">
+        <v>32.4577958475</v>
+      </c>
+      <c r="C47" s="2" t="n">
+        <v>0.2684284051015206</v>
+      </c>
+      <c r="D47" s="2" t="n">
+        <v>-1.942008186948012</v>
+      </c>
+      <c r="E47" s="2" t="n">
+        <v>0.01275518268510964</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;3; BS-&gt;0--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B48" s="2" t="n">
+        <v>3.6194928885</v>
+      </c>
+      <c r="C48" s="2" t="n">
+        <v>0.2073363532005285</v>
+      </c>
+      <c r="D48" s="2" t="n">
+        <v>-1.441647912280093</v>
+      </c>
+      <c r="E48" s="2" t="n">
+        <v>0.3848281287697356</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;3; BS-&gt;1--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B49" s="2" t="n">
+        <v>13.6585438475</v>
+      </c>
+      <c r="C49" s="2" t="n">
+        <v>0.1563776309559063</v>
+      </c>
+      <c r="D49" s="2" t="n">
+        <v>-0.7005743629678314</v>
+      </c>
+      <c r="E49" s="2" t="n">
+        <v>1.104944660183859</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;3; BS-&gt;2--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B50" s="2" t="n">
+        <v>23.805806955</v>
+      </c>
+      <c r="C50" s="2" t="n">
+        <v>0.1662759270462179</v>
+      </c>
+      <c r="D50" s="2" t="n">
+        <v>-1.172215365258637</v>
+      </c>
+      <c r="E50" s="2" t="n">
+        <v>-0.628780069534817</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;3; BS-&gt;3--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B51" s="2" t="n">
+        <v>33.63744504</v>
+      </c>
+      <c r="C51" s="2" t="n">
+        <v>0.253866016495701</v>
+      </c>
+      <c r="D51" s="2" t="n">
+        <v>-1.232302724173985</v>
+      </c>
+      <c r="E51" s="2" t="n">
+        <v>0.340884662534271</v>
       </c>
     </row>
   </sheetData>
@@ -534,7 +1446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -542,11 +1454,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="9.6" customWidth="1" min="1" max="1"/>
+    <col width="24" customWidth="1" min="1" max="1"/>
     <col width="7.199999999999999" customWidth="1" min="2" max="2"/>
     <col width="8.4" customWidth="1" min="3" max="3"/>
     <col width="21.6" customWidth="1" min="4" max="4"/>
-    <col width="21.6" customWidth="1" min="5" max="5"/>
+    <col width="25.2" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -587,35 +1499,1043 @@
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>shapiro</t>
+          <t>omnibus</t>
         </is>
       </c>
       <c r="D2" s="2" t="n">
-        <v>0.9807666540145874</v>
+        <v>0.6418889276599999</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>0.8215728402137756</v>
+        <v>0.72546353933785</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
+          <t>BC-&gt;0--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>0.9507211446762085</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>0.5011969804763794</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;1--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>0.9409359097480774</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>0.360636293888092</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;2--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>0.9569828510284424</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>0.6075426340103149</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;3--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>0.9321847558021545</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>0.2639607489109039</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>BS-&gt;0--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>0.956319272518158</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>0.5958096981048584</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>BS-&gt;1--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>0.9542205929756165</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>0.5593442916870117</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>BS-&gt;2--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>0.8972951173782349</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>0.07275068759918213</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>BS-&gt;3--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>0.9471752643585205</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>0.4463023543357849</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;0; BS-&gt;0--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>0.8921114206314087</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>0.3929412961006165</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;0; BS-&gt;1--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>0.8593451976776123</v>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>0.2578827440738678</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;0; BS-&gt;2--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>0.9494101405143738</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>0.7124338150024414</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;0; BS-&gt;3--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>0.9993059039115906</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>0.9980654120445251</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;1; BS-&gt;0--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>0.9245325326919556</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>0.5626494288444519</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;1; BS-&gt;1--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>0.991174042224884</v>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>0.9634049534797668</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;1; BS-&gt;2--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>0.8144328594207764</v>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>0.1307244449853897</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;1; BS-&gt;3--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>0.9022383093833923</v>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>0.4422619342803955</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;2; BS-&gt;0--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B19" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D19" s="2" t="n">
+        <v>0.927535355091095</v>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>0.5799900889396667</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;2; BS-&gt;1--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C20" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D20" s="2" t="n">
+        <v>0.9358096122741699</v>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>0.6289481520652771</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;2; BS-&gt;2--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D21" s="2" t="n">
+        <v>0.9824661612510681</v>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>0.9163288474082947</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;2; BS-&gt;3--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B22" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D22" s="2" t="n">
+        <v>0.9367258548736572</v>
+      </c>
+      <c r="E22" s="2" t="n">
+        <v>0.6344661712646484</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;3; BS-&gt;0--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B23" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C23" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D23" s="2" t="n">
+        <v>0.9042192697525024</v>
+      </c>
+      <c r="E23" s="2" t="n">
+        <v>0.4523175358772278</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;3; BS-&gt;1--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B24" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D24" s="2" t="n">
+        <v>0.9561636447906494</v>
+      </c>
+      <c r="E24" s="2" t="n">
+        <v>0.7547688484191895</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;3; BS-&gt;2--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B25" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C25" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D25" s="2" t="n">
+        <v>0.9112577438354492</v>
+      </c>
+      <c r="E25" s="2" t="n">
+        <v>0.4890913069248199</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;3; BS-&gt;3--&gt;Time</t>
+        </is>
+      </c>
+      <c r="B26" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D26" s="2" t="n">
+        <v>0.9164301156997681</v>
+      </c>
+      <c r="E26" s="2" t="n">
+        <v>0.5171235799789429</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="inlineStr">
+        <is>
           <t>Speed</t>
         </is>
       </c>
-      <c r="B3" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>shapiro</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="n">
-        <v>0.9591504335403442</v>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>0.2603180110454559</v>
+      <c r="B27" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C27" s="2" t="inlineStr">
+        <is>
+          <t>omnibus</t>
+        </is>
+      </c>
+      <c r="D27" s="2" t="n">
+        <v>29.68663325308417</v>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>3.577910691836292e-07</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;0--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B28" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C28" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D28" s="2" t="n">
+        <v>0.8768904805183411</v>
+      </c>
+      <c r="E28" s="2" t="n">
+        <v>0.0347205325961113</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;1--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B29" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C29" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D29" s="2" t="n">
+        <v>0.8788502216339111</v>
+      </c>
+      <c r="E29" s="2" t="n">
+        <v>0.03723893687129021</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;2--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B30" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C30" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D30" s="2" t="n">
+        <v>0.8822696208953857</v>
+      </c>
+      <c r="E30" s="2" t="n">
+        <v>0.04210183024406433</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;3--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B31" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C31" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D31" s="2" t="n">
+        <v>0.8761458992958069</v>
+      </c>
+      <c r="E31" s="2" t="n">
+        <v>0.03381115198135376</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="inlineStr">
+        <is>
+          <t>BS-&gt;0--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B32" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C32" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D32" s="2" t="n">
+        <v>0.922633171081543</v>
+      </c>
+      <c r="E32" s="2" t="n">
+        <v>0.1859530359506607</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="inlineStr">
+        <is>
+          <t>BS-&gt;1--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B33" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C33" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D33" s="2" t="n">
+        <v>0.9292215704917908</v>
+      </c>
+      <c r="E33" s="2" t="n">
+        <v>0.2369565516710281</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="inlineStr">
+        <is>
+          <t>BS-&gt;2--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B34" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C34" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D34" s="2" t="n">
+        <v>0.9037504196166992</v>
+      </c>
+      <c r="E34" s="2" t="n">
+        <v>0.09230855107307434</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="inlineStr">
+        <is>
+          <t>BS-&gt;3--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B35" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C35" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D35" s="2" t="n">
+        <v>0.9499340057373047</v>
+      </c>
+      <c r="E35" s="2" t="n">
+        <v>0.4886419773101807</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;0; BS-&gt;0--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B36" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C36" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D36" s="2" t="n">
+        <v>0.9354991316795349</v>
+      </c>
+      <c r="E36" s="2" t="n">
+        <v>0.627082347869873</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;0; BS-&gt;1--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B37" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C37" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D37" s="2" t="n">
+        <v>0.8353947401046753</v>
+      </c>
+      <c r="E37" s="2" t="n">
+        <v>0.1823093295097351</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;0; BS-&gt;2--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B38" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C38" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D38" s="2" t="n">
+        <v>0.817193865776062</v>
+      </c>
+      <c r="E38" s="2" t="n">
+        <v>0.1368016600608826</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;0; BS-&gt;3--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B39" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C39" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D39" s="2" t="n">
+        <v>0.9972079992294312</v>
+      </c>
+      <c r="E39" s="2" t="n">
+        <v>0.9906570315361023</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;1; BS-&gt;0--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B40" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C40" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D40" s="2" t="n">
+        <v>0.8870904445648193</v>
+      </c>
+      <c r="E40" s="2" t="n">
+        <v>0.3698038756847382</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;1; BS-&gt;1--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B41" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C41" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D41" s="2" t="n">
+        <v>0.9582235813140869</v>
+      </c>
+      <c r="E41" s="2" t="n">
+        <v>0.7677295207977295</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;1; BS-&gt;2--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B42" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C42" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D42" s="2" t="n">
+        <v>0.7279606461524963</v>
+      </c>
+      <c r="E42" s="2" t="n">
+        <v>0.02348004281520844</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;1; BS-&gt;3--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B43" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C43" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D43" s="2" t="n">
+        <v>0.7828885316848755</v>
+      </c>
+      <c r="E43" s="2" t="n">
+        <v>0.07490747421979904</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;2; BS-&gt;0--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B44" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C44" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D44" s="2" t="n">
+        <v>0.8956226110458374</v>
+      </c>
+      <c r="E44" s="2" t="n">
+        <v>0.4096429347991943</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;2; BS-&gt;1--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B45" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C45" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D45" s="2" t="n">
+        <v>0.921414315700531</v>
+      </c>
+      <c r="E45" s="2" t="n">
+        <v>0.5449044108390808</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;2; BS-&gt;2--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B46" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C46" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D46" s="2" t="n">
+        <v>0.9418443441390991</v>
+      </c>
+      <c r="E46" s="2" t="n">
+        <v>0.6656045913696289</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;2; BS-&gt;3--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B47" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C47" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D47" s="2" t="n">
+        <v>0.827720046043396</v>
+      </c>
+      <c r="E47" s="2" t="n">
+        <v>0.1619345098733902</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;3; BS-&gt;0--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B48" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C48" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D48" s="2" t="n">
+        <v>0.9256935715675354</v>
+      </c>
+      <c r="E48" s="2" t="n">
+        <v>0.5693255662918091</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;3; BS-&gt;1--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B49" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C49" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D49" s="2" t="n">
+        <v>0.7320499420166016</v>
+      </c>
+      <c r="E49" s="2" t="n">
+        <v>0.02584431506693363</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;3; BS-&gt;2--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B50" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C50" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D50" s="2" t="n">
+        <v>0.9065136909484863</v>
+      </c>
+      <c r="E50" s="2" t="n">
+        <v>0.4641272723674774</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="2" t="inlineStr">
+        <is>
+          <t>BC-&gt;3; BS-&gt;3--&gt;Speed</t>
+        </is>
+      </c>
+      <c r="B51" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C51" s="2" t="inlineStr">
+        <is>
+          <t>shapiro</t>
+        </is>
+      </c>
+      <c r="D51" s="2" t="n">
+        <v>0.9797977209091187</v>
+      </c>
+      <c r="E51" s="2" t="n">
+        <v>0.9008312225341797</v>
       </c>
     </row>
   </sheetData>
@@ -639,7 +2559,7 @@
   <cols>
     <col width="12" customWidth="1" min="1" max="1"/>
     <col width="12" customWidth="1" min="2" max="2"/>
-    <col width="20.4" customWidth="1" min="3" max="3"/>
+    <col width="21.6" customWidth="1" min="3" max="3"/>
     <col width="21.6" customWidth="1" min="4" max="4"/>
     <col width="3.6" customWidth="1" min="5" max="5"/>
   </cols>
@@ -681,10 +2601,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>52.29600924913512</v>
+        <v>0.1658117581892244</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>1.099144461992124</v>
+        <v>3.094664763749882</v>
       </c>
       <c r="E2" s="2" t="n">
         <v>5</v>
@@ -700,10 +2620,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>151.6707283106541</v>
+        <v>226.635066551205</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>1.394919974998474</v>
+        <v>-9.340198539599097</v>
       </c>
       <c r="E3" s="2" t="n">
         <v>5</v>
@@ -719,10 +2639,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>4.660459559215026</v>
+        <v>94.38771758086804</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>0.4275316836478985</v>
+        <v>-7.831652199096688</v>
       </c>
       <c r="E4" s="2" t="n">
         <v>5</v>
@@ -738,10 +2658,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>30.71202824765977</v>
+        <v>56.56940767138363</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>0.9512928826271578</v>
+        <v>-6.949973249777518</v>
       </c>
       <c r="E5" s="2" t="n">
         <v>5</v>

</xml_diff>